<commit_message>
17-10-21 class codes pushed
</commit_message>
<xml_diff>
--- a/ML_Unit3/excel/Numerical Examples.xlsx
+++ b/ML_Unit3/excel/Numerical Examples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93c4ddfd9869a0cf/consulting/dono/idma_pt_public/ML_Unit3/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{21447438-AD98-A246-9B8C-D65335E42304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1B011407-EE5C-1146-A307-EC39755B02C4}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{21447438-AD98-A246-9B8C-D65335E42304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B40969DC-51F3-5C49-85B6-A438F3EE354D}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15700" xr2:uid="{B8CF9BDF-FED4-BD4F-A90E-3C7984C95CAB}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15700" activeTab="1" xr2:uid="{B8CF9BDF-FED4-BD4F-A90E-3C7984C95CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Classifier" sheetId="3" r:id="rId1"/>
@@ -4677,7 +4677,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A557BF29-27DE-A84E-AD91-D7CC169E9269}">
   <dimension ref="B24:U52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M27" zoomScale="200" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="C14" zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="T37" sqref="T37"/>
     </sheetView>
   </sheetViews>
@@ -4950,8 +4950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845F3301-0575-2B4D-9771-D8CCAF368F1A}">
   <dimension ref="A3:R19"/>
   <sheetViews>
-    <sheetView zoomScale="164" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4994,17 +4994,17 @@
       </c>
       <c r="D4" s="10">
         <f>Q13</f>
-        <v>17.250000100000001</v>
+        <v>1665.8189172165858</v>
       </c>
       <c r="E4" s="10">
         <f>(C4-D4)^2</f>
-        <v>60.062498449999993</v>
+        <v>2692286.7190958089</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="4">
-        <v>-0.2100127</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -5036,11 +5036,11 @@
         <v>15</v>
       </c>
       <c r="J6" s="4">
-        <v>5.6777870000000004</v>
+        <v>2</v>
       </c>
       <c r="K6" s="9">
         <f>K4+J6*G9+J9*G15</f>
-        <v>474.89220829999999</v>
+        <v>367.76861099999996</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>1</v>
@@ -5090,7 +5090,7 @@
         <v>2</v>
       </c>
       <c r="Q10" s="4">
-        <v>6.2653559999999997</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
@@ -5104,8 +5104,8 @@
         <v>4.5064769</v>
       </c>
       <c r="Q12" s="2">
-        <f>Q10+P12*K7+P15*K19</f>
-        <v>17.250000100000001</v>
+        <f>Q10+P12*K6+P15*K19</f>
+        <v>1665.8189172165858</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>1</v>
@@ -5115,7 +5115,7 @@
       <c r="H13" s="3"/>
       <c r="Q13" s="2">
         <f>Q12</f>
-        <v>17.250000100000001</v>
+        <v>1665.8189172165858</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
added unit 3 and revision session files
</commit_message>
<xml_diff>
--- a/ML_Unit3/excel/Numerical Examples.xlsx
+++ b/ML_Unit3/excel/Numerical Examples.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/93c4ddfd9869a0cf/consulting/dono/idma_pt_public/ML_Unit3/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{21447438-AD98-A246-9B8C-D65335E42304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B40969DC-51F3-5C49-85B6-A438F3EE354D}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{21447438-AD98-A246-9B8C-D65335E42304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15A701E0-2569-544F-A9CC-5454D0BA9017}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15700" activeTab="1" xr2:uid="{B8CF9BDF-FED4-BD4F-A90E-3C7984C95CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Classifier" sheetId="3" r:id="rId1"/>
-    <sheet name="Regression" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="Regression" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="46">
   <si>
     <t>f(z)</t>
   </si>
@@ -105,6 +106,75 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>phi(x) cubic features?</t>
+  </si>
+  <si>
+    <t>(x1,x2,…xn)</t>
+  </si>
+  <si>
+    <t>First Degree</t>
+  </si>
+  <si>
+    <t>x1,x2,x3…xn</t>
+  </si>
+  <si>
+    <t>Second Degree</t>
+  </si>
+  <si>
+    <t>x1^2,x2^2…x1x2,x2x3…</t>
+  </si>
+  <si>
+    <t>Third degree</t>
+  </si>
+  <si>
+    <t>x1^3,x2^2,….x1x2x3,x2x3x4…</t>
+  </si>
+  <si>
+    <t>n1</t>
+  </si>
+  <si>
+    <t>n2</t>
+  </si>
+  <si>
+    <t>n3</t>
+  </si>
+  <si>
+    <t>n1+n2+n3</t>
+  </si>
+  <si>
+    <t>Why?</t>
+  </si>
+  <si>
+    <t>How?</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>d&gt;n</t>
+  </si>
+  <si>
+    <t>It will reduce the number of columns in your data</t>
+  </si>
+  <si>
+    <t>Worse, as good as performing earlier</t>
+  </si>
+  <si>
+    <t>not (x1 AND x1)</t>
+  </si>
+  <si>
+    <t>not (x1 and x1)</t>
+  </si>
+  <si>
+    <t>not (x1)</t>
   </si>
 </sst>
 </file>
@@ -188,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -228,6 +298,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4677,8 +4748,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A557BF29-27DE-A84E-AD91-D7CC169E9269}">
   <dimension ref="B24:U52"/>
   <sheetViews>
-    <sheetView topLeftCell="C14" zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="T37" sqref="T37"/>
+    <sheetView topLeftCell="H19" zoomScale="160" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4947,11 +5018,156 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82D45BB5-BBA6-A544-B6CB-DB87F9E40CA7}">
+  <dimension ref="C1:P19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="L6" s="17">
+        <v>1</v>
+      </c>
+      <c r="M6" s="17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="17">
+        <v>3</v>
+      </c>
+      <c r="M7" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" t="s">
+        <v>41</v>
+      </c>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" t="s">
+        <v>42</v>
+      </c>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+    </row>
+    <row r="15" spans="3:13" x14ac:dyDescent="0.2">
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="19" spans="13:16" x14ac:dyDescent="0.2">
+      <c r="M19" t="s">
+        <v>43</v>
+      </c>
+      <c r="O19" t="s">
+        <v>44</v>
+      </c>
+      <c r="P19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845F3301-0575-2B4D-9771-D8CCAF368F1A}">
   <dimension ref="A3:R19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="164" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView topLeftCell="D1" zoomScale="164" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4994,17 +5210,17 @@
       </c>
       <c r="D4" s="10">
         <f>Q13</f>
-        <v>1665.8189172165858</v>
+        <v>1674.8318710165856</v>
       </c>
       <c r="E4" s="10">
         <f>(C4-D4)^2</f>
-        <v>2692286.7190958089</v>
+        <v>2721945.2026220877</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="K4" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
@@ -5040,7 +5256,7 @@
       </c>
       <c r="K6" s="9">
         <f>K4+J6*G9+J9*G15</f>
-        <v>367.76861099999996</v>
+        <v>369.76861099999996</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>1</v>
@@ -5105,7 +5321,7 @@
       </c>
       <c r="Q12" s="2">
         <f>Q10+P12*K6+P15*K19</f>
-        <v>1665.8189172165858</v>
+        <v>1674.8318710165856</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>1</v>
@@ -5115,7 +5331,7 @@
       <c r="H13" s="3"/>
       <c r="Q13" s="2">
         <f>Q12</f>
-        <v>1665.8189172165858</v>
+        <v>1674.8318710165856</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>3</v>
@@ -5178,7 +5394,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7193503-4A9B-F944-90C9-CFAFBDB828F5}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>